<commit_message>
parquet maker template to create reports subworkflow
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -671,7 +671,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Premature stop codon {'NS1', 'PA-X', 'PB1-F2'}</t>
+          <t>Premature stop codon {'PA-X', 'PB1-F2', 'NS1'}</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Premature stop codon {'NS1', 'PA-X', 'PB1-F2'}</t>
+          <t>Premature stop codon {'PA-X', 'PB1-F2', 'NS1'}</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Premature stop codon {'NS1', 'PA-X', 'PB1-F2'}; Median coverage &lt; 100</t>
+          <t>Premature stop codon {'PA-X', 'PB1-F2', 'NS1'}; Median coverage &lt; 100</t>
         </is>
       </c>
     </row>

</xml_diff>